<commit_message>
subo el dashboard y el exportar a pdf
</commit_message>
<xml_diff>
--- a/proyecto/back/excel/archivo.xlsx
+++ b/proyecto/back/excel/archivo.xlsx
@@ -32,9 +32,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -399,42 +400,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="str">
-        <v>dato</v>
+        <v>marca_temporal</v>
       </c>
       <c r="B1" s="1" t="str">
-        <v>dato1</v>
+        <v>DNI</v>
       </c>
       <c r="C1" s="1" t="str">
-        <v>dato2</v>
+        <v>apellido</v>
       </c>
       <c r="D1" s="1" t="str">
-        <v>dato3</v>
+        <v>nombre</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <v>localidad</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <v>tiene_hermanos</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <v>telefono_alumno</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <v>apellido_tutor</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <v>nombre_tutor</v>
+      </c>
+      <c r="J1" s="1" t="str">
+        <v>telefono_tutor</v>
+      </c>
+      <c r="K1" s="1" t="str">
+        <v>telefono_tutor2</v>
+      </c>
+      <c r="L1" s="1" t="str">
+        <v>curso</v>
+      </c>
+      <c r="M1" s="1" t="str">
+        <v>establecimiento_anio_anterior</v>
+      </c>
+      <c r="N1" s="1" t="str">
+        <v>DNI_tutor</v>
+      </c>
+      <c r="O1" s="1" t="str">
+        <v>cuit_tutor</v>
+      </c>
+      <c r="P1" s="1" t="str">
+        <v>enfermedad_cronica</v>
+      </c>
+      <c r="Q1" s="1" t="str">
+        <v>cual_enfermedad</v>
+      </c>
+      <c r="R1" s="1" t="str">
+        <v>medicacion</v>
+      </c>
+      <c r="S1" s="1" t="str">
+        <v>cual_medicacion</v>
+      </c>
+      <c r="T1" s="1" t="str">
+        <v>correoElectronico</v>
+      </c>
+      <c r="U1" s="1" t="str">
+        <v>fecha_nacimiento</v>
+      </c>
+      <c r="V1" s="1" t="str">
+        <v>edad</v>
+      </c>
+      <c r="W1" s="1" t="str">
+        <v>lugar_nacimiento</v>
+      </c>
+      <c r="X1" s="1" t="str">
+        <v>nacionalidad</v>
+      </c>
+      <c r="Y1" s="1" t="str">
+        <v>domicilio</v>
+      </c>
+      <c r="Z1" s="1" t="str">
+        <v>barrio</v>
+      </c>
+      <c r="AA1" s="1" t="str">
+        <v>cod_postal</v>
+      </c>
+      <c r="AB1" s="1" t="str">
+        <v>materias_adeuda</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v>4</v>
+        <v>iubfrve</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v>5</v>
+        <v>cdoi,cen</v>
       </c>
       <c r="D2" s="1" t="str">
-        <v>7</v>
+        <v>rhuefyn</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <v>iud f</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="G2" s="1" t="str">
+        <v>3i4343</v>
+      </c>
+      <c r="H2" s="1" t="str">
+        <v>vfoi.ju,den</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <v>o dfin</v>
+      </c>
+      <c r="J2" s="1" t="str">
+        <v xml:space="preserve">doinf </v>
+      </c>
+      <c r="K2" s="1" t="str">
+        <v>444444444444444</v>
+      </c>
+      <c r="L2" s="1" t="str">
+        <v>base de datos</v>
+      </c>
+      <c r="M2" s="1" t="str">
+        <v>este colegio</v>
+      </c>
+      <c r="N2" s="1" t="str">
+        <v>urrrr4</v>
+      </c>
+      <c r="O2" s="1" t="str">
+        <v>341093484</v>
+      </c>
+      <c r="P2" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Q2" s="1" t="str">
+        <v>ninguna</v>
+      </c>
+      <c r="R2" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="S2" s="1" t="str">
+        <v>nignuna</v>
+      </c>
+      <c r="T2" s="1" t="str">
+        <v>roro@gmail.com</v>
+      </c>
+      <c r="U2" s="1" t="str">
+        <v>octubre</v>
+      </c>
+      <c r="V2" s="1" t="str">
+        <v>27</v>
+      </c>
+      <c r="W2" s="1" t="str">
+        <v>san martin</v>
+      </c>
+      <c r="X2" s="1" t="str">
+        <v>argentina</v>
+      </c>
+      <c r="Y2" s="1" t="str">
+        <v>constan</v>
+      </c>
+      <c r="Z2" s="1" t="str">
+        <v>eaviucn</v>
+      </c>
+      <c r="AA2" s="1" t="str">
+        <v>1669</v>
+      </c>
+      <c r="AB2" s="1" t="str">
+        <v>No</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AB2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agrego todo lo encargado
</commit_message>
<xml_diff>
--- a/proyecto/back/excel/archivo.xlsx
+++ b/proyecto/back/excel/archivo.xlsx
@@ -32,10 +32,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -400,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -410,85 +409,94 @@
         <v>marca_temporal</v>
       </c>
       <c r="B1" s="1" t="str">
+        <v>foto</v>
+      </c>
+      <c r="C1" s="1" t="str">
         <v>DNI</v>
       </c>
-      <c r="C1" s="1" t="str">
+      <c r="D1" s="1" t="str">
         <v>apellido</v>
       </c>
-      <c r="D1" s="1" t="str">
+      <c r="E1" s="1" t="str">
         <v>nombre</v>
       </c>
-      <c r="E1" s="1" t="str">
+      <c r="F1" s="1" t="str">
         <v>localidad</v>
       </c>
-      <c r="F1" s="1" t="str">
+      <c r="G1" s="1" t="str">
         <v>tiene_hermanos</v>
       </c>
-      <c r="G1" s="1" t="str">
+      <c r="H1" s="1" t="str">
         <v>telefono_alumno</v>
       </c>
-      <c r="H1" s="1" t="str">
+      <c r="I1" s="1" t="str">
         <v>apellido_tutor</v>
       </c>
-      <c r="I1" s="1" t="str">
+      <c r="J1" s="1" t="str">
         <v>nombre_tutor</v>
       </c>
-      <c r="J1" s="1" t="str">
+      <c r="K1" s="1" t="str">
         <v>telefono_tutor</v>
       </c>
-      <c r="K1" s="1" t="str">
+      <c r="L1" s="1" t="str">
         <v>telefono_tutor2</v>
       </c>
-      <c r="L1" s="1" t="str">
+      <c r="M1" s="1" t="str">
         <v>curso</v>
       </c>
-      <c r="M1" s="1" t="str">
+      <c r="N1" s="1" t="str">
         <v>establecimiento_anio_anterior</v>
       </c>
-      <c r="N1" s="1" t="str">
+      <c r="O1" s="1" t="str">
         <v>DNI_tutor</v>
       </c>
-      <c r="O1" s="1" t="str">
+      <c r="P1" s="1" t="str">
         <v>cuit_tutor</v>
       </c>
-      <c r="P1" s="1" t="str">
+      <c r="Q1" s="1" t="str">
         <v>enfermedad_cronica</v>
       </c>
-      <c r="Q1" s="1" t="str">
+      <c r="R1" s="1" t="str">
         <v>cual_enfermedad</v>
       </c>
-      <c r="R1" s="1" t="str">
+      <c r="S1" s="1" t="str">
         <v>medicacion</v>
       </c>
-      <c r="S1" s="1" t="str">
+      <c r="T1" s="1" t="str">
         <v>cual_medicacion</v>
       </c>
-      <c r="T1" s="1" t="str">
+      <c r="U1" s="1" t="str">
         <v>correoElectronico</v>
       </c>
-      <c r="U1" s="1" t="str">
+      <c r="V1" s="1" t="str">
         <v>fecha_nacimiento</v>
       </c>
-      <c r="V1" s="1" t="str">
+      <c r="W1" s="1" t="str">
         <v>edad</v>
       </c>
-      <c r="W1" s="1" t="str">
+      <c r="X1" s="1" t="str">
         <v>lugar_nacimiento</v>
       </c>
-      <c r="X1" s="1" t="str">
+      <c r="Y1" s="1" t="str">
         <v>nacionalidad</v>
       </c>
-      <c r="Y1" s="1" t="str">
+      <c r="Z1" s="1" t="str">
         <v>domicilio</v>
       </c>
-      <c r="Z1" s="1" t="str">
+      <c r="AA1" s="1" t="str">
         <v>barrio</v>
       </c>
-      <c r="AA1" s="1" t="str">
+      <c r="AB1" s="1" t="str">
         <v>cod_postal</v>
       </c>
-      <c r="AB1" s="1" t="str">
+      <c r="AC1" s="1" t="str">
         <v>materias_adeuda</v>
+      </c>
+      <c r="AD1" s="1" t="str">
+        <v>adeuda_materias</v>
+      </c>
+      <c r="AE1" s="1" t="str">
+        <v>quien_aprobo</v>
       </c>
     </row>
     <row r="2">
@@ -496,90 +504,271 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="str">
+        <v>https://cdn.outsideonline.com/wp-content/uploads/2023/03/Funny_Dog_H.jpg?crop=16:9&amp;width=960&amp;enable=upscale&amp;quality=100</v>
+      </c>
+      <c r="C2" s="1" t="str">
         <v>iubfrve</v>
       </c>
-      <c r="C2" s="1" t="str">
+      <c r="D2" s="1" t="str">
         <v>cdoi,cen</v>
       </c>
-      <c r="D2" s="1" t="str">
+      <c r="E2" s="1" t="str">
         <v>rhuefyn</v>
       </c>
-      <c r="E2" s="1" t="str">
+      <c r="F2" s="1" t="str">
         <v>iud f</v>
       </c>
-      <c r="F2" s="1" t="str">
-        <v>No</v>
-      </c>
       <c r="G2" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="H2" s="1" t="str">
         <v>3i4343</v>
       </c>
-      <c r="H2" s="1" t="str">
+      <c r="I2" s="1" t="str">
         <v>vfoi.ju,den</v>
       </c>
-      <c r="I2" s="1" t="str">
+      <c r="J2" s="1" t="str">
         <v>o dfin</v>
       </c>
-      <c r="J2" s="1" t="str">
+      <c r="K2" s="1" t="str">
         <v xml:space="preserve">doinf </v>
       </c>
-      <c r="K2" s="1" t="str">
+      <c r="L2" s="1" t="str">
         <v>444444444444444</v>
       </c>
-      <c r="L2" s="1" t="str">
-        <v>base de datos</v>
-      </c>
       <c r="M2" s="1" t="str">
+        <v>matematica</v>
+      </c>
+      <c r="N2" s="1" t="str">
         <v>este colegio</v>
       </c>
-      <c r="N2" s="1" t="str">
+      <c r="O2" s="1" t="str">
         <v>urrrr4</v>
       </c>
-      <c r="O2" s="1" t="str">
+      <c r="P2" s="1" t="str">
         <v>341093484</v>
       </c>
-      <c r="P2" s="1" t="str">
-        <v>No</v>
-      </c>
       <c r="Q2" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="R2" s="1" t="str">
         <v>ninguna</v>
       </c>
-      <c r="R2" s="1" t="str">
-        <v>No</v>
-      </c>
       <c r="S2" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T2" s="1" t="str">
         <v>nignuna</v>
       </c>
-      <c r="T2" s="1" t="str">
+      <c r="U2" s="1" t="str">
         <v>roro@gmail.com</v>
       </c>
-      <c r="U2" s="1" t="str">
+      <c r="V2" s="1" t="str">
         <v>noviembre</v>
       </c>
-      <c r="V2" s="1" t="str">
+      <c r="W2" s="1" t="str">
         <v>69</v>
       </c>
-      <c r="W2" s="1" t="str">
+      <c r="X2" s="1" t="str">
         <v>san martin</v>
       </c>
-      <c r="X2" s="1" t="str">
+      <c r="Y2" s="1" t="str">
         <v>argentina</v>
       </c>
-      <c r="Y2" s="1" t="str">
+      <c r="Z2" s="1" t="str">
         <v>constan</v>
       </c>
-      <c r="Z2" s="1" t="str">
+      <c r="AA2" s="1" t="str">
         <v>eaviucn</v>
       </c>
-      <c r="AA2" s="1" t="str">
+      <c r="AB2" s="1" t="str">
         <v>1669</v>
       </c>
-      <c r="AB2" s="1" t="str">
+      <c r="AC2" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD2" s="1" t="str">
+        <v>ingles, matematica</v>
+      </c>
+      <c r="AE2" s="1" t="str">
+        <v>susana</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <v>perro</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <v>apellido</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <v>perro</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <v>iud f</v>
+      </c>
+      <c r="G3" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="H3" s="1" t="str">
+        <v>3i4343</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <v>vfoi.ju,den</v>
+      </c>
+      <c r="J3" s="1" t="str">
+        <v>o dfin</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <v xml:space="preserve">doinf </v>
+      </c>
+      <c r="L3" s="1" t="str">
+        <v>444444444444444</v>
+      </c>
+      <c r="M3" s="1" t="str">
+        <v>programacion</v>
+      </c>
+      <c r="N3" s="1" t="str">
+        <v>este colegio</v>
+      </c>
+      <c r="O3" s="1" t="str">
+        <v>urrrr4</v>
+      </c>
+      <c r="P3" s="1" t="str">
+        <v>341093484</v>
+      </c>
+      <c r="Q3" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="R3" s="1" t="str">
+        <v>ninguna</v>
+      </c>
+      <c r="S3" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T3" s="1" t="str">
+        <v>nignuna</v>
+      </c>
+      <c r="U3" s="1" t="str">
+        <v>roro@gmail.com</v>
+      </c>
+      <c r="V3" s="1" t="str">
+        <v>noviembre</v>
+      </c>
+      <c r="W3" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="X3" s="1" t="str">
+        <v>san martin</v>
+      </c>
+      <c r="Y3" s="1" t="str">
+        <v>argentina</v>
+      </c>
+      <c r="Z3" s="1" t="str">
+        <v>constan</v>
+      </c>
+      <c r="AA3" s="1" t="str">
+        <v>eaviucn</v>
+      </c>
+      <c r="AB3" s="1" t="str">
+        <v>1669</v>
+      </c>
+      <c r="AC3" s="1" t="str">
+        <v>No</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>123</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <v>cocina</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <v>gato</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <v>iud f</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="H4" s="1" t="str">
+        <v>3i4343</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <v>vfoi.ju,den</v>
+      </c>
+      <c r="J4" s="1" t="str">
+        <v>o dfin</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <v xml:space="preserve">doinf </v>
+      </c>
+      <c r="L4" s="1" t="str">
+        <v>444444444444444</v>
+      </c>
+      <c r="M4" s="1" t="str">
+        <v>matematica</v>
+      </c>
+      <c r="N4" s="1" t="str">
+        <v>este colegio</v>
+      </c>
+      <c r="O4" s="1" t="str">
+        <v>urrrr4</v>
+      </c>
+      <c r="P4" s="1" t="str">
+        <v>341093484</v>
+      </c>
+      <c r="Q4" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="R4" s="1" t="str">
+        <v>ninguna</v>
+      </c>
+      <c r="S4" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T4" s="1" t="str">
+        <v>nignuna</v>
+      </c>
+      <c r="U4" s="1" t="str">
+        <v>roro@gmail.com</v>
+      </c>
+      <c r="V4" s="1" t="str">
+        <v>noviembre</v>
+      </c>
+      <c r="W4" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="X4" s="1" t="str">
+        <v>san martin</v>
+      </c>
+      <c r="Y4" s="1" t="str">
+        <v>argentina</v>
+      </c>
+      <c r="Z4" s="1" t="str">
+        <v>constan</v>
+      </c>
+      <c r="AA4" s="1" t="str">
+        <v>eaviucn</v>
+      </c>
+      <c r="AB4" s="1" t="str">
+        <v>1669</v>
+      </c>
+      <c r="AC4" s="1" t="str">
         <v>No</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AB2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add alert when adding new data
</commit_message>
<xml_diff>
--- a/proyecto/back/excel/archivo.xlsx
+++ b/proyecto/back/excel/archivo.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE30"/>
+  <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -3112,16 +3112,763 @@
         <v/>
       </c>
     </row>
+    <row r="31">
+      <c r="B31" t="str">
+        <v/>
+      </c>
+      <c r="C31" t="str">
+        <v>442</v>
+      </c>
+      <c r="D31" t="str">
+        <v>qe</v>
+      </c>
+      <c r="E31" t="str">
+        <v>ff</v>
+      </c>
+      <c r="F31" t="str">
+        <v/>
+      </c>
+      <c r="G31" t="str">
+        <v/>
+      </c>
+      <c r="H31" t="str">
+        <v/>
+      </c>
+      <c r="I31" t="str">
+        <v/>
+      </c>
+      <c r="J31" t="str">
+        <v/>
+      </c>
+      <c r="K31" t="str">
+        <v/>
+      </c>
+      <c r="L31" t="str">
+        <v/>
+      </c>
+      <c r="M31" t="str">
+        <v/>
+      </c>
+      <c r="N31" t="str">
+        <v/>
+      </c>
+      <c r="O31" t="str">
+        <v/>
+      </c>
+      <c r="P31" t="str">
+        <v/>
+      </c>
+      <c r="Q31" t="str">
+        <v/>
+      </c>
+      <c r="R31" t="str">
+        <v/>
+      </c>
+      <c r="S31" t="str">
+        <v/>
+      </c>
+      <c r="T31" t="str">
+        <v/>
+      </c>
+      <c r="U31" t="str">
+        <v/>
+      </c>
+      <c r="V31" t="str">
+        <v/>
+      </c>
+      <c r="W31" t="str">
+        <v/>
+      </c>
+      <c r="X31" t="str">
+        <v/>
+      </c>
+      <c r="Y31" t="str">
+        <v/>
+      </c>
+      <c r="Z31" t="str">
+        <v/>
+      </c>
+      <c r="AA31" t="str">
+        <v/>
+      </c>
+      <c r="AB31" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="str">
+        <v/>
+      </c>
+      <c r="C32" t="str">
+        <v>3376</v>
+      </c>
+      <c r="D32" t="str">
+        <v/>
+      </c>
+      <c r="E32" t="str">
+        <v/>
+      </c>
+      <c r="F32" t="str">
+        <v/>
+      </c>
+      <c r="G32" t="str">
+        <v/>
+      </c>
+      <c r="H32" t="str">
+        <v/>
+      </c>
+      <c r="I32" t="str">
+        <v/>
+      </c>
+      <c r="J32" t="str">
+        <v/>
+      </c>
+      <c r="K32" t="str">
+        <v/>
+      </c>
+      <c r="L32" t="str">
+        <v/>
+      </c>
+      <c r="M32" t="str">
+        <v/>
+      </c>
+      <c r="N32" t="str">
+        <v/>
+      </c>
+      <c r="O32" t="str">
+        <v/>
+      </c>
+      <c r="P32" t="str">
+        <v/>
+      </c>
+      <c r="Q32" t="str">
+        <v/>
+      </c>
+      <c r="R32" t="str">
+        <v/>
+      </c>
+      <c r="S32" t="str">
+        <v/>
+      </c>
+      <c r="T32" t="str">
+        <v/>
+      </c>
+      <c r="U32" t="str">
+        <v/>
+      </c>
+      <c r="V32" t="str">
+        <v/>
+      </c>
+      <c r="W32" t="str">
+        <v/>
+      </c>
+      <c r="X32" t="str">
+        <v/>
+      </c>
+      <c r="Y32" t="str">
+        <v/>
+      </c>
+      <c r="Z32" t="str">
+        <v/>
+      </c>
+      <c r="AA32" t="str">
+        <v/>
+      </c>
+      <c r="AB32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="str">
+        <v/>
+      </c>
+      <c r="C33" t="str">
+        <v>gre</v>
+      </c>
+      <c r="D33" t="str">
+        <v/>
+      </c>
+      <c r="E33" t="str">
+        <v/>
+      </c>
+      <c r="F33" t="str">
+        <v/>
+      </c>
+      <c r="G33" t="str">
+        <v/>
+      </c>
+      <c r="H33" t="str">
+        <v/>
+      </c>
+      <c r="I33" t="str">
+        <v/>
+      </c>
+      <c r="J33" t="str">
+        <v/>
+      </c>
+      <c r="K33" t="str">
+        <v/>
+      </c>
+      <c r="L33" t="str">
+        <v/>
+      </c>
+      <c r="M33" t="str">
+        <v/>
+      </c>
+      <c r="N33" t="str">
+        <v/>
+      </c>
+      <c r="O33" t="str">
+        <v/>
+      </c>
+      <c r="P33" t="str">
+        <v/>
+      </c>
+      <c r="Q33" t="str">
+        <v/>
+      </c>
+      <c r="R33" t="str">
+        <v/>
+      </c>
+      <c r="S33" t="str">
+        <v/>
+      </c>
+      <c r="T33" t="str">
+        <v/>
+      </c>
+      <c r="U33" t="str">
+        <v/>
+      </c>
+      <c r="V33" t="str">
+        <v/>
+      </c>
+      <c r="W33" t="str">
+        <v/>
+      </c>
+      <c r="X33" t="str">
+        <v/>
+      </c>
+      <c r="Y33" t="str">
+        <v/>
+      </c>
+      <c r="Z33" t="str">
+        <v/>
+      </c>
+      <c r="AA33" t="str">
+        <v/>
+      </c>
+      <c r="AB33" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="str">
+        <v/>
+      </c>
+      <c r="C34" t="str">
+        <v/>
+      </c>
+      <c r="D34" t="str">
+        <v/>
+      </c>
+      <c r="E34" t="str">
+        <v/>
+      </c>
+      <c r="F34" t="str">
+        <v/>
+      </c>
+      <c r="G34" t="str">
+        <v/>
+      </c>
+      <c r="H34" t="str">
+        <v/>
+      </c>
+      <c r="I34" t="str">
+        <v/>
+      </c>
+      <c r="J34" t="str">
+        <v/>
+      </c>
+      <c r="K34" t="str">
+        <v/>
+      </c>
+      <c r="L34" t="str">
+        <v/>
+      </c>
+      <c r="M34" t="str">
+        <v/>
+      </c>
+      <c r="N34" t="str">
+        <v/>
+      </c>
+      <c r="O34" t="str">
+        <v/>
+      </c>
+      <c r="P34" t="str">
+        <v/>
+      </c>
+      <c r="Q34" t="str">
+        <v/>
+      </c>
+      <c r="R34" t="str">
+        <v/>
+      </c>
+      <c r="S34" t="str">
+        <v/>
+      </c>
+      <c r="T34" t="str">
+        <v/>
+      </c>
+      <c r="U34" t="str">
+        <v/>
+      </c>
+      <c r="V34" t="str">
+        <v/>
+      </c>
+      <c r="W34" t="str">
+        <v/>
+      </c>
+      <c r="X34" t="str">
+        <v/>
+      </c>
+      <c r="Y34" t="str">
+        <v/>
+      </c>
+      <c r="Z34" t="str">
+        <v/>
+      </c>
+      <c r="AA34" t="str">
+        <v/>
+      </c>
+      <c r="AB34" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="str">
+        <v/>
+      </c>
+      <c r="C35" t="str">
+        <v/>
+      </c>
+      <c r="D35" t="str">
+        <v/>
+      </c>
+      <c r="E35" t="str">
+        <v/>
+      </c>
+      <c r="F35" t="str">
+        <v/>
+      </c>
+      <c r="G35" t="str">
+        <v/>
+      </c>
+      <c r="H35" t="str">
+        <v/>
+      </c>
+      <c r="I35" t="str">
+        <v/>
+      </c>
+      <c r="J35" t="str">
+        <v/>
+      </c>
+      <c r="K35" t="str">
+        <v/>
+      </c>
+      <c r="L35" t="str">
+        <v/>
+      </c>
+      <c r="M35" t="str">
+        <v/>
+      </c>
+      <c r="N35" t="str">
+        <v/>
+      </c>
+      <c r="O35" t="str">
+        <v/>
+      </c>
+      <c r="P35" t="str">
+        <v/>
+      </c>
+      <c r="Q35" t="str">
+        <v/>
+      </c>
+      <c r="R35" t="str">
+        <v/>
+      </c>
+      <c r="S35" t="str">
+        <v/>
+      </c>
+      <c r="T35" t="str">
+        <v/>
+      </c>
+      <c r="U35" t="str">
+        <v/>
+      </c>
+      <c r="V35" t="str">
+        <v/>
+      </c>
+      <c r="W35" t="str">
+        <v/>
+      </c>
+      <c r="X35" t="str">
+        <v/>
+      </c>
+      <c r="Y35" t="str">
+        <v/>
+      </c>
+      <c r="Z35" t="str">
+        <v/>
+      </c>
+      <c r="AA35" t="str">
+        <v/>
+      </c>
+      <c r="AB35" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="str">
+        <v/>
+      </c>
+      <c r="C36" t="str">
+        <v/>
+      </c>
+      <c r="D36" t="str">
+        <v/>
+      </c>
+      <c r="E36" t="str">
+        <v/>
+      </c>
+      <c r="F36" t="str">
+        <v/>
+      </c>
+      <c r="G36" t="str">
+        <v/>
+      </c>
+      <c r="H36" t="str">
+        <v/>
+      </c>
+      <c r="I36" t="str">
+        <v/>
+      </c>
+      <c r="J36" t="str">
+        <v/>
+      </c>
+      <c r="K36" t="str">
+        <v/>
+      </c>
+      <c r="L36" t="str">
+        <v/>
+      </c>
+      <c r="M36" t="str">
+        <v/>
+      </c>
+      <c r="N36" t="str">
+        <v/>
+      </c>
+      <c r="O36" t="str">
+        <v/>
+      </c>
+      <c r="P36" t="str">
+        <v/>
+      </c>
+      <c r="Q36" t="str">
+        <v/>
+      </c>
+      <c r="R36" t="str">
+        <v/>
+      </c>
+      <c r="S36" t="str">
+        <v/>
+      </c>
+      <c r="T36" t="str">
+        <v/>
+      </c>
+      <c r="U36" t="str">
+        <v/>
+      </c>
+      <c r="V36" t="str">
+        <v/>
+      </c>
+      <c r="W36" t="str">
+        <v/>
+      </c>
+      <c r="X36" t="str">
+        <v/>
+      </c>
+      <c r="Y36" t="str">
+        <v/>
+      </c>
+      <c r="Z36" t="str">
+        <v/>
+      </c>
+      <c r="AA36" t="str">
+        <v/>
+      </c>
+      <c r="AB36" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="str">
+        <v/>
+      </c>
+      <c r="C37" t="str">
+        <v/>
+      </c>
+      <c r="D37" t="str">
+        <v/>
+      </c>
+      <c r="E37" t="str">
+        <v/>
+      </c>
+      <c r="F37" t="str">
+        <v/>
+      </c>
+      <c r="G37" t="str">
+        <v/>
+      </c>
+      <c r="H37" t="str">
+        <v/>
+      </c>
+      <c r="I37" t="str">
+        <v/>
+      </c>
+      <c r="J37" t="str">
+        <v/>
+      </c>
+      <c r="K37" t="str">
+        <v/>
+      </c>
+      <c r="L37" t="str">
+        <v/>
+      </c>
+      <c r="M37" t="str">
+        <v/>
+      </c>
+      <c r="N37" t="str">
+        <v/>
+      </c>
+      <c r="O37" t="str">
+        <v/>
+      </c>
+      <c r="P37" t="str">
+        <v/>
+      </c>
+      <c r="Q37" t="str">
+        <v/>
+      </c>
+      <c r="R37" t="str">
+        <v/>
+      </c>
+      <c r="S37" t="str">
+        <v/>
+      </c>
+      <c r="T37" t="str">
+        <v/>
+      </c>
+      <c r="U37" t="str">
+        <v/>
+      </c>
+      <c r="V37" t="str">
+        <v/>
+      </c>
+      <c r="W37" t="str">
+        <v/>
+      </c>
+      <c r="X37" t="str">
+        <v/>
+      </c>
+      <c r="Y37" t="str">
+        <v/>
+      </c>
+      <c r="Z37" t="str">
+        <v/>
+      </c>
+      <c r="AA37" t="str">
+        <v/>
+      </c>
+      <c r="AB37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="str">
+        <v/>
+      </c>
+      <c r="C38" t="str">
+        <v/>
+      </c>
+      <c r="D38" t="str">
+        <v/>
+      </c>
+      <c r="E38" t="str">
+        <v/>
+      </c>
+      <c r="F38" t="str">
+        <v/>
+      </c>
+      <c r="G38" t="str">
+        <v/>
+      </c>
+      <c r="H38" t="str">
+        <v/>
+      </c>
+      <c r="I38" t="str">
+        <v/>
+      </c>
+      <c r="J38" t="str">
+        <v/>
+      </c>
+      <c r="K38" t="str">
+        <v/>
+      </c>
+      <c r="L38" t="str">
+        <v/>
+      </c>
+      <c r="M38" t="str">
+        <v/>
+      </c>
+      <c r="N38" t="str">
+        <v/>
+      </c>
+      <c r="O38" t="str">
+        <v/>
+      </c>
+      <c r="P38" t="str">
+        <v/>
+      </c>
+      <c r="Q38" t="str">
+        <v/>
+      </c>
+      <c r="R38" t="str">
+        <v/>
+      </c>
+      <c r="S38" t="str">
+        <v/>
+      </c>
+      <c r="T38" t="str">
+        <v/>
+      </c>
+      <c r="U38" t="str">
+        <v/>
+      </c>
+      <c r="V38" t="str">
+        <v/>
+      </c>
+      <c r="W38" t="str">
+        <v/>
+      </c>
+      <c r="X38" t="str">
+        <v/>
+      </c>
+      <c r="Y38" t="str">
+        <v/>
+      </c>
+      <c r="Z38" t="str">
+        <v/>
+      </c>
+      <c r="AA38" t="str">
+        <v/>
+      </c>
+      <c r="AB38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="str">
+        <v/>
+      </c>
+      <c r="C39" t="str">
+        <v>42</v>
+      </c>
+      <c r="D39" t="str">
+        <v/>
+      </c>
+      <c r="E39" t="str">
+        <v/>
+      </c>
+      <c r="F39" t="str">
+        <v/>
+      </c>
+      <c r="G39" t="str">
+        <v/>
+      </c>
+      <c r="H39" t="str">
+        <v/>
+      </c>
+      <c r="I39" t="str">
+        <v/>
+      </c>
+      <c r="J39" t="str">
+        <v/>
+      </c>
+      <c r="K39" t="str">
+        <v/>
+      </c>
+      <c r="L39" t="str">
+        <v/>
+      </c>
+      <c r="M39" t="str">
+        <v/>
+      </c>
+      <c r="N39" t="str">
+        <v/>
+      </c>
+      <c r="O39" t="str">
+        <v/>
+      </c>
+      <c r="P39" t="str">
+        <v/>
+      </c>
+      <c r="Q39" t="str">
+        <v/>
+      </c>
+      <c r="R39" t="str">
+        <v/>
+      </c>
+      <c r="S39" t="str">
+        <v/>
+      </c>
+      <c r="T39" t="str">
+        <v/>
+      </c>
+      <c r="U39" t="str">
+        <v/>
+      </c>
+      <c r="V39" t="str">
+        <v/>
+      </c>
+      <c r="W39" t="str">
+        <v/>
+      </c>
+      <c r="X39" t="str">
+        <v/>
+      </c>
+      <c r="Y39" t="str">
+        <v/>
+      </c>
+      <c r="Z39" t="str">
+        <v/>
+      </c>
+      <c r="AA39" t="str">
+        <v/>
+      </c>
+      <c r="AB39" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE30"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE39"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -3411,9 +4158,55 @@
         <v>er</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>3345214</v>
+      </c>
+      <c r="B13" t="str">
+        <v/>
+      </c>
+      <c r="C13" t="str">
+        <v>qqqqq</v>
+      </c>
+      <c r="E13" t="str">
+        <v>matematica</v>
+      </c>
+      <c r="F13" t="str">
+        <v>3</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Desaprobado</v>
+      </c>
+      <c r="H13" t="str">
+        <v>4to</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>442</v>
+      </c>
+      <c r="B14" t="str">
+        <v>qe</v>
+      </c>
+      <c r="C14" t="str">
+        <v>ff</v>
+      </c>
+      <c r="E14" t="str">
+        <v>fr</v>
+      </c>
+      <c r="F14" t="str">
+        <v>5</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Aprobado</v>
+      </c>
+      <c r="H14" t="str">
+        <v>wvwfwfqf</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added seconds the user
</commit_message>
<xml_diff>
--- a/proyecto/back/excel/archivo.xlsx
+++ b/proyecto/back/excel/archivo.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE45"/>
+  <dimension ref="A1:AE46"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -4357,17 +4357,99 @@
         <v/>
       </c>
     </row>
+    <row r="46">
+      <c r="B46" t="str">
+        <v>https://cdn.outsideonline.com/wp-content/uploads/2023/03/Funny_Dog_H.jpg?crop=16:9&amp;width=960&amp;enable=upscale&amp;quality=100</v>
+      </c>
+      <c r="C46" t="str">
+        <v>3825533188</v>
+      </c>
+      <c r="D46" t="str">
+        <v>movil</v>
+      </c>
+      <c r="E46" t="str">
+        <v>paqueta</v>
+      </c>
+      <c r="F46" t="str">
+        <v/>
+      </c>
+      <c r="G46" t="str">
+        <v/>
+      </c>
+      <c r="H46" t="str">
+        <v/>
+      </c>
+      <c r="I46" t="str">
+        <v/>
+      </c>
+      <c r="J46" t="str">
+        <v/>
+      </c>
+      <c r="K46" t="str">
+        <v/>
+      </c>
+      <c r="L46" t="str">
+        <v/>
+      </c>
+      <c r="M46" t="str">
+        <v/>
+      </c>
+      <c r="N46" t="str">
+        <v/>
+      </c>
+      <c r="O46" t="str">
+        <v/>
+      </c>
+      <c r="P46" t="str">
+        <v/>
+      </c>
+      <c r="Q46" t="str">
+        <v/>
+      </c>
+      <c r="R46" t="str">
+        <v/>
+      </c>
+      <c r="S46" t="str">
+        <v/>
+      </c>
+      <c r="T46" t="str">
+        <v/>
+      </c>
+      <c r="U46" t="str">
+        <v/>
+      </c>
+      <c r="V46" t="str">
+        <v/>
+      </c>
+      <c r="W46" t="str">
+        <v/>
+      </c>
+      <c r="X46" t="str">
+        <v/>
+      </c>
+      <c r="Y46" t="str">
+        <v/>
+      </c>
+      <c r="Z46" t="str">
+        <v/>
+      </c>
+      <c r="AA46" t="str">
+        <v/>
+      </c>
+      <c r="AB46" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE45"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE46"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -4739,9 +4821,32 @@
         <v>43</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>3825533188</v>
+      </c>
+      <c r="B18" t="str">
+        <v>movil</v>
+      </c>
+      <c r="C18" t="str">
+        <v>paqueta</v>
+      </c>
+      <c r="D18" t="str">
+        <v>matematica</v>
+      </c>
+      <c r="E18" t="str">
+        <v>6</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Desaprobado</v>
+      </c>
+      <c r="G18" t="str">
+        <v>4to</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>